<commit_message>
Moved to local names
</commit_message>
<xml_diff>
--- a/online-kalkulator-print-addon/Template.xlsx
+++ b/online-kalkulator-print-addon/Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scherzer Thomas\Documents\GitHub\hassio-addons\online-kalkulator-print-addon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B5173C-40C3-418C-9302-06ACBB88AE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFCFA9E-965D-488F-9223-9E264C9EEBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,66 +17,66 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arbeitsverfahren!$A$3:$F$69</definedName>
-    <definedName name="GK_LeistungsbereichMax">Arbeitsverfahren!$D$87</definedName>
-    <definedName name="GK_LeistungsbereichMin">Arbeitsverfahren!$C$87</definedName>
-    <definedName name="GK_NebenzeitenGrundmaschine">Arbeitsverfahren!$D$75</definedName>
-    <definedName name="GK_NebenzeitenPersonal">Arbeitsverfahren!$D$74</definedName>
-    <definedName name="GK_OrganisationsUnternehmenskosten">Arbeitsverfahren!$D$79</definedName>
-    <definedName name="GK_Personalkosten">Arbeitsverfahren!$E$71</definedName>
-    <definedName name="GK_Wagnis">Arbeitsverfahren!$D$82</definedName>
-    <definedName name="GM_Anschaffungspreis">Arbeitsverfahren!$D$5</definedName>
-    <definedName name="GM_GebuehrenRel">Arbeitsverfahren!$C$28</definedName>
-    <definedName name="GM_Jahresstunden">Arbeitsverfahren!$D$8</definedName>
-    <definedName name="GM_MieteAbs">Arbeitsverfahren!$D$27</definedName>
-    <definedName name="GM_Name">Arbeitsverfahren!$C$4</definedName>
-    <definedName name="GM_Nutzungsdauer">Arbeitsverfahren!$D$9</definedName>
-    <definedName name="GM_ReparaturenRel">Arbeitsverfahren!$C$53</definedName>
-    <definedName name="GM_Restwert">Arbeitsverfahren!$D$6</definedName>
-    <definedName name="GM_SchmierstoffKosten">Arbeitsverfahren!$D$52</definedName>
-    <definedName name="GM_SchmierstoffVerbrauch">Arbeitsverfahren!$C$52</definedName>
-    <definedName name="GM_SonstigesKosten">Arbeitsverfahren!$D$54</definedName>
-    <definedName name="GM_SonstigesVerbrauch">Arbeitsverfahren!$C$54</definedName>
-    <definedName name="GM_TreibstoffKosten">Arbeitsverfahren!$D$51</definedName>
-    <definedName name="GM_TreibstoffVerbrauch">Arbeitsverfahren!$C$51</definedName>
-    <definedName name="GM_UnterbringungRel">Arbeitsverfahren!$C$30</definedName>
-    <definedName name="GM_VersicherungRel">Arbeitsverfahren!$C$29</definedName>
-    <definedName name="GM_Zinssatz">Arbeitsverfahren!$D$7</definedName>
-    <definedName name="M1_Aktiv">Arbeitsverfahren!$A$11:$A$15,Arbeitsverfahren!$A$32:$A$39,Arbeitsverfahren!$A$56:$A$61</definedName>
-    <definedName name="M1_Anschaffungspreis">Arbeitsverfahren!$D$11</definedName>
-    <definedName name="M1_GebuehrenRel">Arbeitsverfahren!$C$36</definedName>
-    <definedName name="M1_Jahresstunden">Arbeitsverfahren!$D$14</definedName>
-    <definedName name="M1_MieteAbs">Arbeitsverfahren!$D$35</definedName>
-    <definedName name="M1_Name">Arbeitsverfahren!$C$10</definedName>
-    <definedName name="M1_Nutzungsdauer">Arbeitsverfahren!$D$15</definedName>
-    <definedName name="M1_ReparaturenRel">Arbeitsverfahren!$C$59</definedName>
-    <definedName name="M1_Restwert">Arbeitsverfahren!$D$12</definedName>
-    <definedName name="M1_SchmierstoffKosten">Arbeitsverfahren!$D$58</definedName>
-    <definedName name="M1_SchmierstoffVerbrauch">Arbeitsverfahren!$C$58</definedName>
-    <definedName name="M1_SonstigesKosten">Arbeitsverfahren!$D$60</definedName>
-    <definedName name="M1_SonstigesVerbrauch">Arbeitsverfahren!$C$60</definedName>
-    <definedName name="M1_TreibstoffKosten">Arbeitsverfahren!$D$57</definedName>
-    <definedName name="M1_TreibstoffVerbrauch">Arbeitsverfahren!$C$57</definedName>
-    <definedName name="M1_UnterbringungRel">Arbeitsverfahren!$C$38</definedName>
-    <definedName name="M1_VersicherungRel">Arbeitsverfahren!$C$37</definedName>
-    <definedName name="M1_Zinssatz">Arbeitsverfahren!$D$13</definedName>
-    <definedName name="M2_Aktiv">Arbeitsverfahren!$A$17:$A$21,Arbeitsverfahren!$A$40:$A$47,Arbeitsverfahren!$A$62:$A$67</definedName>
-    <definedName name="M2_Anschaffungspreis">Arbeitsverfahren!$D$17</definedName>
-    <definedName name="M2_GebuehrenRel">Arbeitsverfahren!$C$44</definedName>
-    <definedName name="M2_Jahresstunden">Arbeitsverfahren!$D$20</definedName>
-    <definedName name="M2_MieteAbs">Arbeitsverfahren!$D$43</definedName>
-    <definedName name="M2_Name">Arbeitsverfahren!$C$16</definedName>
-    <definedName name="M2_Nutzungsdauer">Arbeitsverfahren!$D$21</definedName>
-    <definedName name="M2_ReparaturenRel">Arbeitsverfahren!$C$65</definedName>
-    <definedName name="M2_Restwert">Arbeitsverfahren!$D$18</definedName>
-    <definedName name="M2_SchmierstoffKosten">Arbeitsverfahren!$D$64</definedName>
-    <definedName name="M2_SchmierstoffVerbrauch">Arbeitsverfahren!$C$64</definedName>
-    <definedName name="M2_SonstigesKosten">Arbeitsverfahren!$D$66</definedName>
-    <definedName name="M2_SonstigesVerbrauch">Arbeitsverfahren!$C$66</definedName>
-    <definedName name="M2_TreibstoffKosten">Arbeitsverfahren!$D$63</definedName>
-    <definedName name="M2_TreibstoffVerbrauch">Arbeitsverfahren!$C$63</definedName>
-    <definedName name="M2_UnterbringungRel">Arbeitsverfahren!$C$46</definedName>
-    <definedName name="M2_VersicherungRel">Arbeitsverfahren!$C$45</definedName>
-    <definedName name="M2_Zinssatz">Arbeitsverfahren!$D$19</definedName>
+    <definedName name="GK_LeistungsbereichMax" localSheetId="0">Arbeitsverfahren!$D$87</definedName>
+    <definedName name="GK_LeistungsbereichMin" localSheetId="0">Arbeitsverfahren!$C$87</definedName>
+    <definedName name="GK_NebenzeitenGrundmaschine" localSheetId="0">Arbeitsverfahren!$D$75</definedName>
+    <definedName name="GK_NebenzeitenPersonal" localSheetId="0">Arbeitsverfahren!$D$74</definedName>
+    <definedName name="GK_OrganisationsUnternehmenskosten" localSheetId="0">Arbeitsverfahren!$D$79</definedName>
+    <definedName name="GK_Personalkosten" localSheetId="0">Arbeitsverfahren!$E$71</definedName>
+    <definedName name="GK_Wagnis" localSheetId="0">Arbeitsverfahren!$D$82</definedName>
+    <definedName name="GM_Anschaffungspreis" localSheetId="0">Arbeitsverfahren!$D$5</definedName>
+    <definedName name="GM_GebuehrenRel" localSheetId="0">Arbeitsverfahren!$C$28</definedName>
+    <definedName name="GM_Jahresstunden" localSheetId="0">Arbeitsverfahren!$D$8</definedName>
+    <definedName name="GM_MieteAbs" localSheetId="0">Arbeitsverfahren!$D$27</definedName>
+    <definedName name="GM_Name" localSheetId="0">Arbeitsverfahren!$C$4</definedName>
+    <definedName name="GM_Nutzungsdauer" localSheetId="0">Arbeitsverfahren!$D$9</definedName>
+    <definedName name="GM_ReparaturenRel" localSheetId="0">Arbeitsverfahren!$C$53</definedName>
+    <definedName name="GM_Restwert" localSheetId="0">Arbeitsverfahren!$D$6</definedName>
+    <definedName name="GM_SchmierstoffKosten" localSheetId="0">Arbeitsverfahren!$D$52</definedName>
+    <definedName name="GM_SchmierstoffVerbrauch" localSheetId="0">Arbeitsverfahren!$C$52</definedName>
+    <definedName name="GM_SonstigesKosten" localSheetId="0">Arbeitsverfahren!$D$54</definedName>
+    <definedName name="GM_SonstigesVerbrauch" localSheetId="0">Arbeitsverfahren!$C$54</definedName>
+    <definedName name="GM_TreibstoffKosten" localSheetId="0">Arbeitsverfahren!$D$51</definedName>
+    <definedName name="GM_TreibstoffVerbrauch" localSheetId="0">Arbeitsverfahren!$C$51</definedName>
+    <definedName name="GM_UnterbringungRel" localSheetId="0">Arbeitsverfahren!$C$30</definedName>
+    <definedName name="GM_VersicherungRel" localSheetId="0">Arbeitsverfahren!$C$29</definedName>
+    <definedName name="GM_Zinssatz" localSheetId="0">Arbeitsverfahren!$D$7</definedName>
+    <definedName name="M1_Aktiv" localSheetId="0">Arbeitsverfahren!$A$11:$A$15,Arbeitsverfahren!$A$32:$A$39,Arbeitsverfahren!$A$56:$A$61</definedName>
+    <definedName name="M1_Anschaffungspreis" localSheetId="0">Arbeitsverfahren!$D$11</definedName>
+    <definedName name="M1_GebuehrenRel" localSheetId="0">Arbeitsverfahren!$C$36</definedName>
+    <definedName name="M1_Jahresstunden" localSheetId="0">Arbeitsverfahren!$D$14</definedName>
+    <definedName name="M1_MieteAbs" localSheetId="0">Arbeitsverfahren!$D$35</definedName>
+    <definedName name="M1_Name" localSheetId="0">Arbeitsverfahren!$C$10</definedName>
+    <definedName name="M1_Nutzungsdauer" localSheetId="0">Arbeitsverfahren!$D$15</definedName>
+    <definedName name="M1_ReparaturenRel" localSheetId="0">Arbeitsverfahren!$C$59</definedName>
+    <definedName name="M1_Restwert" localSheetId="0">Arbeitsverfahren!$D$12</definedName>
+    <definedName name="M1_SchmierstoffKosten" localSheetId="0">Arbeitsverfahren!$D$58</definedName>
+    <definedName name="M1_SchmierstoffVerbrauch" localSheetId="0">Arbeitsverfahren!$C$58</definedName>
+    <definedName name="M1_SonstigesKosten" localSheetId="0">Arbeitsverfahren!$D$60</definedName>
+    <definedName name="M1_SonstigesVerbrauch" localSheetId="0">Arbeitsverfahren!$C$60</definedName>
+    <definedName name="M1_TreibstoffKosten" localSheetId="0">Arbeitsverfahren!$D$57</definedName>
+    <definedName name="M1_TreibstoffVerbrauch" localSheetId="0">Arbeitsverfahren!$C$57</definedName>
+    <definedName name="M1_UnterbringungRel" localSheetId="0">Arbeitsverfahren!$C$38</definedName>
+    <definedName name="M1_VersicherungRel" localSheetId="0">Arbeitsverfahren!$C$37</definedName>
+    <definedName name="M1_Zinssatz" localSheetId="0">Arbeitsverfahren!$D$13</definedName>
+    <definedName name="M2_Aktiv" localSheetId="0">Arbeitsverfahren!$A$17:$A$21,Arbeitsverfahren!$A$40:$A$47,Arbeitsverfahren!$A$62:$A$67</definedName>
+    <definedName name="M2_Anschaffungspreis" localSheetId="0">Arbeitsverfahren!$D$17</definedName>
+    <definedName name="M2_GebuehrenRel" localSheetId="0">Arbeitsverfahren!$C$44</definedName>
+    <definedName name="M2_Jahresstunden" localSheetId="0">Arbeitsverfahren!$D$20</definedName>
+    <definedName name="M2_MieteAbs" localSheetId="0">Arbeitsverfahren!$D$43</definedName>
+    <definedName name="M2_Name" localSheetId="0">Arbeitsverfahren!$C$16</definedName>
+    <definedName name="M2_Nutzungsdauer" localSheetId="0">Arbeitsverfahren!$D$21</definedName>
+    <definedName name="M2_ReparaturenRel" localSheetId="0">Arbeitsverfahren!$C$65</definedName>
+    <definedName name="M2_Restwert" localSheetId="0">Arbeitsverfahren!$D$18</definedName>
+    <definedName name="M2_SchmierstoffKosten" localSheetId="0">Arbeitsverfahren!$D$64</definedName>
+    <definedName name="M2_SchmierstoffVerbrauch" localSheetId="0">Arbeitsverfahren!$C$64</definedName>
+    <definedName name="M2_SonstigesKosten" localSheetId="0">Arbeitsverfahren!$D$66</definedName>
+    <definedName name="M2_SonstigesVerbrauch" localSheetId="0">Arbeitsverfahren!$C$66</definedName>
+    <definedName name="M2_TreibstoffKosten" localSheetId="0">Arbeitsverfahren!$D$63</definedName>
+    <definedName name="M2_TreibstoffVerbrauch" localSheetId="0">Arbeitsverfahren!$C$63</definedName>
+    <definedName name="M2_UnterbringungRel" localSheetId="0">Arbeitsverfahren!$C$46</definedName>
+    <definedName name="M2_VersicherungRel" localSheetId="0">Arbeitsverfahren!$C$45</definedName>
+    <definedName name="M2_Zinssatz" localSheetId="0">Arbeitsverfahren!$D$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -588,6 +588,9 @@
     <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -611,9 +614,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -940,13 +940,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr codeName="Tabelle1" filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -985,19 +985,19 @@
       <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="101"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="101"/>
+      <c r="A5" s="94"/>
       <c r="B5" s="19" t="s">
         <v>56</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="101"/>
+      <c r="A6" s="94"/>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="101"/>
+      <c r="A7" s="94"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="101"/>
+      <c r="A8" s="94"/>
       <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
@@ -1051,7 +1051,7 @@
       <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="101"/>
+      <c r="A9" s="94"/>
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
@@ -1068,19 +1068,19 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="101"/>
+      <c r="A10" s="94"/>
       <c r="B10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="97" t="s">
+      <c r="C10" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="101" t="str">
+      <c r="A11" s="94" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1097,7 +1097,7 @@
       <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="101" t="str">
+      <c r="A12" s="94" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="101" t="str">
+      <c r="A13" s="94" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="101" t="str">
+      <c r="A14" s="94" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="101" t="str">
+      <c r="A15" s="94" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1166,19 +1166,19 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="101"/>
+      <c r="A16" s="94"/>
       <c r="B16" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="99"/>
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="101" t="str">
+      <c r="A17" s="94" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1195,7 +1195,7 @@
       <c r="F17" s="45"/>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="101" t="str">
+      <c r="A18" s="94" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="F18" s="45"/>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="101" t="str">
+      <c r="A19" s="94" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="F19" s="45"/>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="101" t="str">
+      <c r="A20" s="94" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="F20" s="45"/>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="101" t="str">
+      <c r="A21" s="94" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1292,13 +1292,13 @@
       <c r="B24" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="99" t="str">
+      <c r="C24" s="100" t="str">
         <f>GM_Name</f>
         <v xml:space="preserve">Traktor 150 PS </v>
       </c>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="99"/>
+      <c r="D24" s="100"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="100"/>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" s="72"/>
@@ -1311,7 +1311,7 @@
         <v>6250</v>
       </c>
       <c r="E25" s="25">
-        <f>IF(GM_Jahresstunden=0,0,D25/GM_Jahresstunden)</f>
+        <f t="shared" ref="E25:E30" si="0">IF(GM_Jahresstunden=0,0,D25/GM_Jahresstunden)</f>
         <v>10.416666666666666</v>
       </c>
       <c r="F25" s="19" t="s">
@@ -1329,7 +1329,7 @@
         <v>3375</v>
       </c>
       <c r="E26" s="25">
-        <f>IF(GM_Jahresstunden=0,0,D26/GM_Jahresstunden)</f>
+        <f t="shared" si="0"/>
         <v>5.625</v>
       </c>
       <c r="F26" s="19" t="s">
@@ -1346,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="25">
-        <f>IF(GM_Jahresstunden=0,0,D27/GM_Jahresstunden)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F27" s="19" t="s">
@@ -1366,7 +1366,7 @@
         <v>150</v>
       </c>
       <c r="E28" s="25">
-        <f>IF(GM_Jahresstunden=0,0,D28/GM_Jahresstunden)</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="F28" s="19" t="s">
@@ -1386,7 +1386,7 @@
         <v>450</v>
       </c>
       <c r="E29" s="25">
-        <f>IF(GM_Jahresstunden=0,0,D29/GM_Jahresstunden)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="F29" s="19" t="s">
@@ -1406,7 +1406,7 @@
         <v>750</v>
       </c>
       <c r="E30" s="25">
-        <f>IF(GM_Jahresstunden=0,0,D30/GM_Jahresstunden)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
       <c r="F30" s="19" t="s">
@@ -1432,24 +1432,24 @@
       </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A32" s="94" t="str">
+        <f t="shared" ref="A32:A39" si="1">IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
       <c r="B32" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="100" t="str">
+      <c r="C32" s="101" t="str">
         <f>M1_Name</f>
         <v>Kreiselegge 3m</v>
       </c>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A33" s="94" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B33" s="34" t="s">
@@ -1461,7 +1461,7 @@
         <v>600</v>
       </c>
       <c r="E33" s="40">
-        <f>IF(M1_Jahresstunden=0,0,D33/M1_Jahresstunden)</f>
+        <f t="shared" ref="E33:E38" si="2">IF(M1_Jahresstunden=0,0,D33/M1_Jahresstunden)</f>
         <v>7.5</v>
       </c>
       <c r="F33" s="34" t="s">
@@ -1469,8 +1469,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A34" s="94" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B34" s="34" t="s">
@@ -1482,7 +1482,7 @@
         <v>280</v>
       </c>
       <c r="E34" s="40">
-        <f>IF(M1_Jahresstunden=0,0,D34/M1_Jahresstunden)</f>
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
       <c r="F34" s="34" t="s">
@@ -1490,8 +1490,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A35" s="94" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B35" s="34" t="s">
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="40">
-        <f>IF(M1_Jahresstunden=0,0,D35/M1_Jahresstunden)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F35" s="34" t="s">
@@ -1510,8 +1510,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A36" s="94" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B36" s="34" t="s">
@@ -1525,7 +1525,7 @@
         <v>20</v>
       </c>
       <c r="E36" s="40">
-        <f>IF(M1_Jahresstunden=0,0,D36/M1_Jahresstunden)</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="F36" s="34" t="s">
@@ -1533,8 +1533,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A37" s="94" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B37" s="34" t="s">
@@ -1548,7 +1548,7 @@
         <v>60</v>
       </c>
       <c r="E37" s="40">
-        <f>IF(M1_Jahresstunden=0,0,D37/M1_Jahresstunden)</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="F37" s="34" t="s">
@@ -1556,8 +1556,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A38" s="94" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B38" s="34" t="s">
@@ -1571,7 +1571,7 @@
         <v>100</v>
       </c>
       <c r="E38" s="40">
-        <f>IF(M1_Jahresstunden=0,0,D38/M1_Jahresstunden)</f>
+        <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
       <c r="F38" s="34" t="s">
@@ -1579,8 +1579,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A39" s="94" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B39" s="34" t="s">
@@ -1600,24 +1600,24 @@
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A40" s="94" t="str">
+        <f t="shared" ref="A40:A47" si="3">IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
       <c r="B40" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="94" t="str">
+      <c r="C40" s="95" t="str">
         <f>M2_Name</f>
         <v>Sämaschine 3m</v>
       </c>
-      <c r="D40" s="94"/>
-      <c r="E40" s="94"/>
-      <c r="F40" s="94"/>
+      <c r="D40" s="95"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="95"/>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A41" s="94" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B41" s="45" t="s">
@@ -1629,7 +1629,7 @@
         <v>500</v>
       </c>
       <c r="E41" s="51">
-        <f>IF(M2_Jahresstunden=0,0,D41/M2_Jahresstunden)</f>
+        <f t="shared" ref="E41:E46" si="4">IF(M2_Jahresstunden=0,0,D41/M2_Jahresstunden)</f>
         <v>10</v>
       </c>
       <c r="F41" s="45" t="s">
@@ -1637,8 +1637,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A42" s="94" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B42" s="45" t="s">
@@ -1650,7 +1650,7 @@
         <v>260</v>
       </c>
       <c r="E42" s="51">
-        <f>IF(M2_Jahresstunden=0,0,D42/M2_Jahresstunden)</f>
+        <f t="shared" si="4"/>
         <v>5.2</v>
       </c>
       <c r="F42" s="45" t="s">
@@ -1658,8 +1658,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A43" s="94" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B43" s="45" t="s">
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="51">
-        <f>IF(M2_Jahresstunden=0,0,D43/M2_Jahresstunden)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F43" s="45" t="s">
@@ -1678,8 +1678,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A44" s="94" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B44" s="45" t="s">
@@ -1693,7 +1693,7 @@
         <v>18</v>
       </c>
       <c r="E44" s="51">
-        <f>IF(M2_Jahresstunden=0,0,D44/M2_Jahresstunden)</f>
+        <f t="shared" si="4"/>
         <v>0.36</v>
       </c>
       <c r="F44" s="45" t="s">
@@ -1701,8 +1701,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A45" s="94" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B45" s="45" t="s">
@@ -1716,7 +1716,7 @@
         <v>54</v>
       </c>
       <c r="E45" s="51">
-        <f>IF(M2_Jahresstunden=0,0,D45/M2_Jahresstunden)</f>
+        <f t="shared" si="4"/>
         <v>1.08</v>
       </c>
       <c r="F45" s="45" t="s">
@@ -1724,8 +1724,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A46" s="94" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B46" s="45" t="s">
@@ -1739,7 +1739,7 @@
         <v>90</v>
       </c>
       <c r="E46" s="51">
-        <f>IF(M2_Jahresstunden=0,0,D46/M2_Jahresstunden)</f>
+        <f t="shared" si="4"/>
         <v>1.8</v>
       </c>
       <c r="F46" s="45" t="s">
@@ -1747,8 +1747,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A47" s="94" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B47" s="45" t="s">
@@ -1808,13 +1808,13 @@
       <c r="B50" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="99" t="str">
+      <c r="C50" s="100" t="str">
         <f>GM_Name</f>
         <v xml:space="preserve">Traktor 150 PS </v>
       </c>
-      <c r="D50" s="99"/>
-      <c r="E50" s="99"/>
-      <c r="F50" s="99"/>
+      <c r="D50" s="100"/>
+      <c r="E50" s="100"/>
+      <c r="F50" s="100"/>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A51" s="72"/>
@@ -1847,7 +1847,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25">
-        <f t="shared" ref="E52:E54" si="0">C52*D52</f>
+        <f t="shared" ref="E52:E54" si="5">C52*D52</f>
         <v>0.8</v>
       </c>
       <c r="F52" s="19" t="s">
@@ -1886,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F54" s="19" t="s">
@@ -1909,24 +1909,24 @@
       </c>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A56" s="94" t="str">
+        <f t="shared" ref="A56:A61" si="6">IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
       <c r="B56" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="100" t="str">
+      <c r="C56" s="101" t="str">
         <f>M1_Name</f>
         <v>Kreiselegge 3m</v>
       </c>
-      <c r="D56" s="100"/>
-      <c r="E56" s="100"/>
-      <c r="F56" s="100"/>
+      <c r="D56" s="101"/>
+      <c r="E56" s="101"/>
+      <c r="F56" s="101"/>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A57" s="94" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B57" s="34" t="s">
@@ -1947,8 +1947,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A58" s="94" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B58" s="34" t="s">
@@ -1961,7 +1961,7 @@
         <v>4</v>
       </c>
       <c r="E58" s="40">
-        <f t="shared" ref="E58:E60" si="1">C58*D58</f>
+        <f t="shared" ref="E58:E60" si="7">C58*D58</f>
         <v>0.8</v>
       </c>
       <c r="F58" s="34" t="s">
@@ -1969,8 +1969,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A59" s="94" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B59" s="34" t="s">
@@ -1992,8 +1992,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A60" s="94" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B60" s="34" t="s">
@@ -2006,7 +2006,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F60" s="34" t="s">
@@ -2014,8 +2014,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="101" t="str">
-        <f>IF(ISBLANK(M1_Name),NA(),"")</f>
+      <c r="A61" s="94" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="B61" s="34" t="s">
@@ -2032,24 +2032,24 @@
       </c>
     </row>
     <row r="62" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A62" s="94" t="str">
+        <f t="shared" ref="A62:A67" si="8">IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
       <c r="B62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="94" t="str">
+      <c r="C62" s="95" t="str">
         <f>M2_Name</f>
         <v>Sämaschine 3m</v>
       </c>
-      <c r="D62" s="94"/>
-      <c r="E62" s="94"/>
-      <c r="F62" s="94"/>
+      <c r="D62" s="95"/>
+      <c r="E62" s="95"/>
+      <c r="F62" s="95"/>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A63" s="94" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="B63" s="45" t="s">
@@ -2070,8 +2070,8 @@
       </c>
     </row>
     <row r="64" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A64" s="94" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="B64" s="45" t="s">
@@ -2084,7 +2084,7 @@
         <v>4</v>
       </c>
       <c r="E64" s="51">
-        <f t="shared" ref="E64:E66" si="2">C64*D64</f>
+        <f t="shared" ref="E64:E66" si="9">C64*D64</f>
         <v>0.8</v>
       </c>
       <c r="F64" s="45" t="s">
@@ -2092,8 +2092,8 @@
       </c>
     </row>
     <row r="65" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A65" s="94" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="B65" s="45" t="s">
@@ -2115,8 +2115,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A66" s="94" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="B66" s="45" t="s">
@@ -2129,7 +2129,7 @@
         <v>1</v>
       </c>
       <c r="E66" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F66" s="45" t="s">
@@ -2137,8 +2137,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="101" t="str">
-        <f>IF(ISBLANK(M2_Name),NA(),"")</f>
+      <c r="A67" s="94" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="B67" s="45" t="s">
@@ -2444,11 +2444,11 @@
         <v>174.45781249999999</v>
       </c>
       <c r="D88" s="89">
-        <f t="shared" ref="D88:E88" si="3">$E$84/D87</f>
+        <f t="shared" ref="D88:E88" si="10">$E$84/D87</f>
         <v>107.35865384615384</v>
       </c>
       <c r="E88" s="89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>132.92023809523809</v>
       </c>
       <c r="F88" s="75" t="s">
@@ -2477,14 +2477,14 @@
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="C56:F56"/>
   </mergeCells>
-  <conditionalFormatting sqref="A22:E22 A16:B16 A1:F15 A17:F21 A23:F88">
+  <conditionalFormatting sqref="A22:E22 A23:F88">
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>CELL("Schutz",A1)=0</formula>
+      <formula>CELL("Schutz",A22)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:F16">
+  <conditionalFormatting sqref="A1:F21">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>CELL("Schutz",C16)=0</formula>
+      <formula>CELL("Schutz",A1)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Minor changes in excel file
</commit_message>
<xml_diff>
--- a/online-kalkulator-print-addon/Template.xlsx
+++ b/online-kalkulator-print-addon/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scherzer Thomas\Documents\GitHub\hassio-addons\online-kalkulator-print-addon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFCFA9E-965D-488F-9223-9E264C9EEBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB9BCBD-29D6-49FE-893A-7467437043D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27250" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsverfahren" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,6 @@
     <xf numFmtId="4" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -616,6 +615,7 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -945,8 +945,8 @@
   </sheetPr>
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -956,7 +956,7 @@
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -968,16 +968,16 @@
       <c r="B2" s="10"/>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="69" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="31"/>
-      <c r="D3" s="92">
+      <c r="D3" s="91">
         <f ca="1">TODAY()</f>
-        <v>46021</v>
+        <v>46026</v>
       </c>
       <c r="E3" s="31" t="s">
         <v>9</v>
@@ -985,19 +985,19 @@
       <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="94"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="94"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="19" t="s">
         <v>56</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="94"/>
+      <c r="A6" s="93"/>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="94"/>
+      <c r="A7" s="93"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="94"/>
+      <c r="A8" s="93"/>
       <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
@@ -1051,7 +1051,7 @@
       <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="94"/>
+      <c r="A9" s="93"/>
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
@@ -1068,19 +1068,19 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="94"/>
+      <c r="A10" s="93"/>
       <c r="B10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="98" t="s">
+      <c r="C10" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="94" t="str">
+      <c r="A11" s="93" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1097,7 +1097,7 @@
       <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="94" t="str">
+      <c r="A12" s="93" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="94" t="str">
+      <c r="A13" s="93" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="94" t="str">
+      <c r="A14" s="93" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="94" t="str">
+      <c r="A15" s="93" t="str">
         <f>IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1166,19 +1166,19 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="94"/>
+      <c r="A16" s="93"/>
       <c r="B16" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="99" t="s">
+      <c r="C16" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="94" t="str">
+      <c r="A17" s="93" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1195,7 +1195,7 @@
       <c r="F17" s="45"/>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="94" t="str">
+      <c r="A18" s="93" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="F18" s="45"/>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="94" t="str">
+      <c r="A19" s="93" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="F19" s="45"/>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="94" t="str">
+      <c r="A20" s="93" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="F20" s="45"/>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="94" t="str">
+      <c r="A21" s="93" t="str">
         <f>IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
@@ -1266,11 +1266,11 @@
     <row r="22" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="8"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="93"/>
+      <c r="D22" s="92"/>
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="69" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="30" t="s">
@@ -1279,7 +1279,7 @@
       <c r="C23" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="71" t="s">
+      <c r="D23" s="70" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="32" t="s">
@@ -1288,20 +1288,20 @@
       <c r="F23" s="31"/>
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="72"/>
+      <c r="A24" s="71"/>
       <c r="B24" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="100" t="str">
+      <c r="C24" s="99" t="str">
         <f>GM_Name</f>
         <v xml:space="preserve">Traktor 150 PS </v>
       </c>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="100"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="72"/>
+      <c r="A25" s="71"/>
       <c r="B25" s="19" t="s">
         <v>20</v>
       </c>
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="72"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="19" t="s">
         <v>21</v>
       </c>
@@ -1337,7 +1337,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="72"/>
+      <c r="A27" s="71"/>
       <c r="B27" s="19" t="s">
         <v>26</v>
       </c>
@@ -1354,7 +1354,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="72"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="19" t="s">
         <v>23</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="72"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="19" t="s">
         <v>22</v>
       </c>
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="72"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="19" t="s">
         <v>2</v>
       </c>
@@ -1414,7 +1414,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="72"/>
+      <c r="A31" s="71"/>
       <c r="B31" s="19" t="s">
         <v>27</v>
       </c>
@@ -1432,23 +1432,23 @@
       </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="94" t="str">
+      <c r="A32" s="93" t="str">
         <f t="shared" ref="A32:A39" si="1">IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
       <c r="B32" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="101" t="str">
+      <c r="C32" s="100" t="str">
         <f>M1_Name</f>
         <v>Kreiselegge 3m</v>
       </c>
-      <c r="D32" s="101"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="101"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="100"/>
+      <c r="F32" s="100"/>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="94" t="str">
+      <c r="A33" s="93" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="94" t="str">
+      <c r="A34" s="93" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1490,7 +1490,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="94" t="str">
+      <c r="A35" s="93" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1510,7 +1510,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="94" t="str">
+      <c r="A36" s="93" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="94" t="str">
+      <c r="A37" s="93" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1556,7 +1556,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="94" t="str">
+      <c r="A38" s="93" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="94" t="str">
+      <c r="A39" s="93" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1600,23 +1600,23 @@
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="94" t="str">
+      <c r="A40" s="93" t="str">
         <f t="shared" ref="A40:A47" si="3">IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
       <c r="B40" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="95" t="str">
+      <c r="C40" s="94" t="str">
         <f>M2_Name</f>
         <v>Sämaschine 3m</v>
       </c>
-      <c r="D40" s="95"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="95"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="94"/>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="94" t="str">
+      <c r="A41" s="93" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1637,7 +1637,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="94" t="str">
+      <c r="A42" s="93" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1658,7 +1658,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="94" t="str">
+      <c r="A43" s="93" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1678,7 +1678,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="94" t="str">
+      <c r="A44" s="93" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1701,7 +1701,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="94" t="str">
+      <c r="A45" s="93" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="94" t="str">
+      <c r="A46" s="93" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1747,7 +1747,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="94" t="str">
+      <c r="A47" s="93" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1768,16 +1768,16 @@
       </c>
     </row>
     <row r="48" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="70"/>
+      <c r="A48" s="69"/>
       <c r="B48" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C48" s="30"/>
-      <c r="D48" s="86">
+      <c r="D48" s="85">
         <f>D31+D39+D47</f>
         <v>12957</v>
       </c>
-      <c r="E48" s="91">
+      <c r="E48" s="90">
         <f>E31+E39+E47</f>
         <v>49.981666666666669</v>
       </c>
@@ -1786,7 +1786,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A49" s="70" t="s">
+      <c r="A49" s="69" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="30" t="s">
@@ -1795,29 +1795,29 @@
       <c r="C49" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D49" s="71" t="s">
+      <c r="D49" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="71" t="s">
+      <c r="E49" s="70" t="s">
         <v>25</v>
       </c>
       <c r="F49" s="31"/>
     </row>
     <row r="50" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="72"/>
+      <c r="A50" s="71"/>
       <c r="B50" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="100" t="str">
+      <c r="C50" s="99" t="str">
         <f>GM_Name</f>
         <v xml:space="preserve">Traktor 150 PS </v>
       </c>
-      <c r="D50" s="100"/>
-      <c r="E50" s="100"/>
-      <c r="F50" s="100"/>
+      <c r="D50" s="99"/>
+      <c r="E50" s="99"/>
+      <c r="F50" s="99"/>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="72"/>
+      <c r="A51" s="71"/>
       <c r="B51" s="19" t="s">
         <v>30</v>
       </c>
@@ -1836,7 +1836,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="72"/>
+      <c r="A52" s="71"/>
       <c r="B52" s="19" t="s">
         <v>31</v>
       </c>
@@ -1855,7 +1855,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="72"/>
+      <c r="A53" s="71"/>
       <c r="B53" s="19" t="s">
         <v>44</v>
       </c>
@@ -1875,7 +1875,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="72"/>
+      <c r="A54" s="71"/>
       <c r="B54" s="19" t="s">
         <v>32</v>
       </c>
@@ -1894,7 +1894,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="72"/>
+      <c r="A55" s="71"/>
       <c r="B55" s="19" t="s">
         <v>33</v>
       </c>
@@ -1909,23 +1909,23 @@
       </c>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="94" t="str">
+      <c r="A56" s="93" t="str">
         <f t="shared" ref="A56:A61" si="6">IF(ISBLANK(M1_Name),NA(),"")</f>
         <v/>
       </c>
       <c r="B56" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="101" t="str">
+      <c r="C56" s="100" t="str">
         <f>M1_Name</f>
         <v>Kreiselegge 3m</v>
       </c>
-      <c r="D56" s="101"/>
-      <c r="E56" s="101"/>
-      <c r="F56" s="101"/>
+      <c r="D56" s="100"/>
+      <c r="E56" s="100"/>
+      <c r="F56" s="100"/>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="94" t="str">
+      <c r="A57" s="93" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="94" t="str">
+      <c r="A58" s="93" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="94" t="str">
+      <c r="A59" s="93" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -1992,7 +1992,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="94" t="str">
+      <c r="A60" s="93" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -2014,7 +2014,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="94" t="str">
+      <c r="A61" s="93" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -2032,23 +2032,23 @@
       </c>
     </row>
     <row r="62" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="94" t="str">
+      <c r="A62" s="93" t="str">
         <f t="shared" ref="A62:A67" si="8">IF(ISBLANK(M2_Name),NA(),"")</f>
         <v/>
       </c>
       <c r="B62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="95" t="str">
+      <c r="C62" s="94" t="str">
         <f>M2_Name</f>
         <v>Sämaschine 3m</v>
       </c>
-      <c r="D62" s="95"/>
-      <c r="E62" s="95"/>
-      <c r="F62" s="95"/>
+      <c r="D62" s="94"/>
+      <c r="E62" s="94"/>
+      <c r="F62" s="94"/>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="94" t="str">
+      <c r="A63" s="93" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -2070,7 +2070,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="94" t="str">
+      <c r="A64" s="93" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="94" t="str">
+      <c r="A65" s="93" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -2115,7 +2115,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="94" t="str">
+      <c r="A66" s="93" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -2137,7 +2137,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="94" t="str">
+      <c r="A67" s="93" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -2155,13 +2155,13 @@
       </c>
     </row>
     <row r="68" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="70"/>
+      <c r="A68" s="69"/>
       <c r="B68" s="30" t="s">
         <v>35</v>
       </c>
       <c r="C68" s="30"/>
-      <c r="D68" s="86"/>
-      <c r="E68" s="91">
+      <c r="D68" s="85"/>
+      <c r="E68" s="90">
         <f>E55+E61+E67</f>
         <v>38.06</v>
       </c>
@@ -2170,15 +2170,15 @@
       </c>
     </row>
     <row r="69" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="70" t="s">
+      <c r="A69" s="69" t="s">
         <v>55</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C69" s="30"/>
-      <c r="D69" s="86"/>
-      <c r="E69" s="91">
+      <c r="D69" s="85"/>
+      <c r="E69" s="90">
         <f>E48+E68</f>
         <v>88.041666666666671</v>
       </c>
@@ -2236,18 +2236,18 @@
       <c r="B74" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C74" s="59">
+      <c r="C74" s="101">
         <f>1/(1+GK_NebenzeitenPersonal)</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="D74" s="60">
+      <c r="D74" s="59">
         <v>0.4</v>
       </c>
-      <c r="E74" s="61">
+      <c r="E74" s="60">
         <f>GK_Personalkosten*GK_NebenzeitenPersonal</f>
         <v>7.2</v>
       </c>
-      <c r="F74" s="62" t="s">
+      <c r="F74" s="61" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2256,18 +2256,18 @@
       <c r="B75" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C75" s="59">
+      <c r="C75" s="101">
         <f>1/(1+GK_NebenzeitenGrundmaschine)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="D75" s="60">
+      <c r="D75" s="59">
         <v>0.2</v>
       </c>
-      <c r="E75" s="61">
+      <c r="E75" s="60">
         <f>($E$55+$E$31)*D75</f>
         <v>10.418333333333333</v>
       </c>
-      <c r="F75" s="62" t="s">
+      <c r="F75" s="61" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2277,12 +2277,12 @@
         <v>59</v>
       </c>
       <c r="C76" s="56"/>
-      <c r="D76" s="80"/>
-      <c r="E76" s="90">
+      <c r="D76" s="79"/>
+      <c r="E76" s="89">
         <f>SUM(E74:E75)</f>
         <v>17.618333333333332</v>
       </c>
-      <c r="F76" s="81" t="s">
+      <c r="F76" s="80" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2290,40 +2290,40 @@
       <c r="A77" s="11"/>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
-      <c r="D77" s="87"/>
+      <c r="D77" s="86"/>
       <c r="E77" s="17"/>
-      <c r="F77" s="88"/>
+      <c r="F77" s="87"/>
     </row>
     <row r="78" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A78" s="63" t="s">
+      <c r="A78" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="63" t="s">
+      <c r="B78" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="C78" s="64"/>
-      <c r="D78" s="65" t="s">
+      <c r="C78" s="63"/>
+      <c r="D78" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="E78" s="66" t="s">
+      <c r="E78" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="F78" s="67"/>
+      <c r="F78" s="66"/>
     </row>
     <row r="79" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A79" s="64"/>
-      <c r="B79" s="68" t="s">
+      <c r="A79" s="63"/>
+      <c r="B79" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="C79" s="68"/>
-      <c r="D79" s="69">
+      <c r="C79" s="67"/>
+      <c r="D79" s="68">
         <v>0.12</v>
       </c>
-      <c r="E79" s="66">
+      <c r="E79" s="65">
         <f>GK_OrganisationsUnternehmenskosten*($E$69+GK_Personalkosten)</f>
         <v>12.725</v>
       </c>
-      <c r="F79" s="67" t="s">
+      <c r="F79" s="66" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2334,35 +2334,35 @@
       <c r="F80" s="14"/>
     </row>
     <row r="81" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A81" s="63" t="s">
+      <c r="A81" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="73" t="s">
+      <c r="B81" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="C81" s="68"/>
-      <c r="D81" s="65" t="s">
+      <c r="C81" s="67"/>
+      <c r="D81" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="E81" s="66" t="s">
+      <c r="E81" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="F81" s="67"/>
+      <c r="F81" s="66"/>
     </row>
     <row r="82" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A82" s="64"/>
-      <c r="B82" s="68" t="s">
+      <c r="A82" s="63"/>
+      <c r="B82" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="C82" s="68"/>
-      <c r="D82" s="69">
+      <c r="C82" s="67"/>
+      <c r="D82" s="68">
         <v>0.03</v>
       </c>
-      <c r="E82" s="66">
+      <c r="E82" s="65">
         <f>GK_Wagnis*($E$69+GK_Personalkosten)</f>
         <v>3.1812499999999999</v>
       </c>
-      <c r="F82" s="68" t="s">
+      <c r="F82" s="67" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2370,24 +2370,24 @@
       <c r="A83" s="11"/>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
-      <c r="D83" s="87"/>
+      <c r="D83" s="86"/>
       <c r="E83" s="17"/>
-      <c r="F83" s="88"/>
+      <c r="F83" s="87"/>
     </row>
     <row r="84" spans="1:6" s="4" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="74" t="s">
+      <c r="A84" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B84" s="75" t="s">
+      <c r="B84" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C84" s="75"/>
-      <c r="D84" s="76"/>
-      <c r="E84" s="89">
+      <c r="C84" s="74"/>
+      <c r="D84" s="75"/>
+      <c r="E84" s="88">
         <f>$E$69+GK_Personalkosten+$E$76+$E$79+$E$82</f>
         <v>139.56625</v>
       </c>
-      <c r="F84" s="75" t="s">
+      <c r="F84" s="74" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2397,61 +2397,61 @@
       <c r="E85" s="17"/>
     </row>
     <row r="86" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A86" s="74" t="s">
+      <c r="A86" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="B86" s="75" t="s">
+      <c r="B86" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="C86" s="77" t="s">
+      <c r="C86" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="D86" s="78" t="s">
+      <c r="D86" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="E86" s="79" t="s">
+      <c r="E86" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="F86" s="75"/>
+      <c r="F86" s="74"/>
     </row>
     <row r="87" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A87" s="82"/>
-      <c r="B87" s="77" t="s">
+      <c r="A87" s="81"/>
+      <c r="B87" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="C87" s="83">
+      <c r="C87" s="82">
         <v>0.8</v>
       </c>
-      <c r="D87" s="83">
+      <c r="D87" s="82">
         <v>1.3</v>
       </c>
-      <c r="E87" s="84">
+      <c r="E87" s="83">
         <f>AVERAGE(C87:D87)</f>
         <v>1.05</v>
       </c>
-      <c r="F87" s="85">
+      <c r="F87" s="84">
         <f>AVEDEV(C87:D87)/E87</f>
         <v>0.23809523809523808</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="4" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="74"/>
-      <c r="B88" s="75" t="s">
+      <c r="A88" s="73"/>
+      <c r="B88" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="C88" s="89">
+      <c r="C88" s="88">
         <f>$E$84/C87</f>
         <v>174.45781249999999</v>
       </c>
-      <c r="D88" s="89">
+      <c r="D88" s="88">
         <f t="shared" ref="D88:E88" si="10">$E$84/D87</f>
         <v>107.35865384615384</v>
       </c>
-      <c r="E88" s="89">
+      <c r="E88" s="88">
         <f t="shared" si="10"/>
         <v>132.92023809523809</v>
       </c>
-      <c r="F88" s="75" t="s">
+      <c r="F88" s="74" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2488,9 +2488,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;LSeite &amp;P/&amp;N&amp;CONLINE-KALKULATOR LAND- UND FORSTWIRTSCHAFTLICHE ARBEITSVERFAHREN&amp;R&amp;D</oddHeader>
+    <oddHeader>&amp;LSeite &amp;P/&amp;N&amp;Cwww.online-kalkulator.at&amp;R&amp;D</oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="48" max="16383" man="1"/>

</xml_diff>

<commit_message>
Added units to description texts in excel
</commit_message>
<xml_diff>
--- a/online-kalkulator-print-addon/Template.xlsx
+++ b/online-kalkulator-print-addon/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scherzer Thomas\Documents\GitHub\hassio-addons\online-kalkulator-print-addon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BC8AFD-16FC-4F2B-A819-E23AA1FE9BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7C80D8-C1DA-4170-9CAA-6A24CD5D0DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27250" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsverfahren" sheetId="1" r:id="rId1"/>
@@ -189,12 +189,6 @@
     <t xml:space="preserve">Variable Maschinenkosten: </t>
   </si>
   <si>
-    <t>Treibstoffe (l/Std.)</t>
-  </si>
-  <si>
-    <t>Schmierstoffkosten</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige Kosten </t>
   </si>
   <si>
@@ -301,6 +295,12 @@
   </si>
   <si>
     <t>Schwankung</t>
+  </si>
+  <si>
+    <t>Treibstoffe (l/h)</t>
+  </si>
+  <si>
+    <t>Schmierstoffkosten (l/h)</t>
   </si>
 </sst>
 </file>
@@ -314,7 +314,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="&quot;±&quot;0%"/>
     <numFmt numFmtId="169" formatCode="&quot;Ø &quot;0.0"/>
-    <numFmt numFmtId="171" formatCode="&quot;Σ:&quot;\ #,##0&quot; h&quot;"/>
+    <numFmt numFmtId="170" formatCode="&quot;Σ:&quot;\ #,##0&quot; h&quot;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -590,6 +590,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -614,36 +644,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -975,7 +975,7 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I86" sqref="I86"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -990,7 +990,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -998,7 +998,7 @@
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="67" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>19</v>
@@ -1006,7 +1006,7 @@
       <c r="C3" s="31"/>
       <c r="D3" s="86">
         <f ca="1">TODAY()</f>
-        <v>46026</v>
+        <v>46038</v>
       </c>
       <c r="E3" s="31" t="s">
         <v>9</v>
@@ -1018,17 +1018,17 @@
       <c r="B4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="88"/>
       <c r="B5" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="20">
@@ -1077,7 +1077,7 @@
       <c r="E8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="97">
+      <c r="F8" s="90">
         <f>D9*D8</f>
         <v>10800</v>
       </c>
@@ -1101,12 +1101,12 @@
       <c r="B10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="93" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
+      <c r="C10" s="105" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="88" t="str">
@@ -1114,7 +1114,7 @@
         <v/>
       </c>
       <c r="B11" s="33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="34">
@@ -1172,7 +1172,7 @@
       <c r="E14" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="98">
+      <c r="F14" s="91">
         <f>D15*D14</f>
         <v>1600</v>
       </c>
@@ -1199,12 +1199,12 @@
       <c r="B16" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="94" t="s">
+      <c r="C16" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="94"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="88" t="str">
@@ -1212,7 +1212,7 @@
         <v/>
       </c>
       <c r="B17" s="44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" s="44"/>
       <c r="D17" s="45">
@@ -1270,7 +1270,7 @@
       <c r="E20" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="99">
+      <c r="F20" s="92">
         <f>D21*D20</f>
         <v>1000</v>
       </c>
@@ -1305,13 +1305,13 @@
       <c r="B23" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="100" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="101" t="s">
+      <c r="C23" s="93" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="102" t="s">
+      <c r="E23" s="95" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="31"/>
@@ -1321,13 +1321,13 @@
       <c r="B24" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="95" t="str">
+      <c r="C24" s="107" t="str">
         <f>GM_Name</f>
         <v xml:space="preserve">Traktor 150 PS </v>
       </c>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
+      <c r="D24" s="107"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="107"/>
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" s="68"/>
@@ -1468,13 +1468,13 @@
       <c r="B32" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="96" t="str">
+      <c r="C32" s="108" t="str">
         <f>M1_Name</f>
         <v>Kreiselegge 3m</v>
       </c>
-      <c r="D32" s="96"/>
-      <c r="E32" s="96"/>
-      <c r="F32" s="96"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="108"/>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A33" s="88" t="str">
@@ -1636,13 +1636,13 @@
       <c r="B40" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="90" t="str">
+      <c r="C40" s="102" t="str">
         <f>M2_Name</f>
         <v>Sämaschine 3m</v>
       </c>
-      <c r="D40" s="90"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="90"/>
+      <c r="D40" s="102"/>
+      <c r="E40" s="102"/>
+      <c r="F40" s="102"/>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A41" s="88" t="str">
@@ -1799,7 +1799,7 @@
     <row r="48" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="67"/>
       <c r="B48" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C48" s="30"/>
       <c r="D48" s="80">
@@ -1821,13 +1821,13 @@
       <c r="B49" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="100" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="101" t="s">
-        <v>43</v>
-      </c>
-      <c r="E49" s="101" t="s">
+      <c r="C49" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" s="94" t="s">
         <v>25</v>
       </c>
       <c r="F49" s="31"/>
@@ -1837,18 +1837,18 @@
       <c r="B50" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="95" t="str">
+      <c r="C50" s="107" t="str">
         <f>GM_Name</f>
         <v xml:space="preserve">Traktor 150 PS </v>
       </c>
-      <c r="D50" s="95"/>
-      <c r="E50" s="95"/>
-      <c r="F50" s="95"/>
+      <c r="D50" s="107"/>
+      <c r="E50" s="107"/>
+      <c r="F50" s="107"/>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A51" s="68"/>
       <c r="B51" s="19" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C51" s="27">
         <v>15</v>
@@ -1867,7 +1867,7 @@
     <row r="52" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A52" s="68"/>
       <c r="B52" s="19" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C52" s="27">
         <v>0.2</v>
@@ -1886,7 +1886,7 @@
     <row r="53" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A53" s="68"/>
       <c r="B53" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C53" s="29">
         <v>0.7</v>
@@ -1906,7 +1906,7 @@
     <row r="54" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A54" s="68"/>
       <c r="B54" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C54" s="27">
         <v>0</v>
@@ -1925,7 +1925,7 @@
     <row r="55" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A55" s="68"/>
       <c r="B55" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="25"/>
@@ -1945,13 +1945,13 @@
       <c r="B56" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="96" t="str">
+      <c r="C56" s="108" t="str">
         <f>M1_Name</f>
         <v>Kreiselegge 3m</v>
       </c>
-      <c r="D56" s="96"/>
-      <c r="E56" s="96"/>
-      <c r="F56" s="96"/>
+      <c r="D56" s="108"/>
+      <c r="E56" s="108"/>
+      <c r="F56" s="108"/>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A57" s="88" t="str">
@@ -1959,7 +1959,7 @@
         <v/>
       </c>
       <c r="B57" s="33" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C57" s="41">
         <v>0</v>
@@ -1981,7 +1981,7 @@
         <v/>
       </c>
       <c r="B58" s="33" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C58" s="41">
         <v>0.2</v>
@@ -2003,7 +2003,7 @@
         <v/>
       </c>
       <c r="B59" s="33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C59" s="42">
         <v>0.7</v>
@@ -2026,7 +2026,7 @@
         <v/>
       </c>
       <c r="B60" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C60" s="41">
         <v>0</v>
@@ -2048,7 +2048,7 @@
         <v/>
       </c>
       <c r="B61" s="33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C61" s="33"/>
       <c r="D61" s="39"/>
@@ -2068,13 +2068,13 @@
       <c r="B62" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="90" t="str">
+      <c r="C62" s="102" t="str">
         <f>M2_Name</f>
         <v>Sämaschine 3m</v>
       </c>
-      <c r="D62" s="90"/>
-      <c r="E62" s="90"/>
-      <c r="F62" s="90"/>
+      <c r="D62" s="102"/>
+      <c r="E62" s="102"/>
+      <c r="F62" s="102"/>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A63" s="88" t="str">
@@ -2082,7 +2082,7 @@
         <v/>
       </c>
       <c r="B63" s="44" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C63" s="52">
         <v>0</v>
@@ -2104,7 +2104,7 @@
         <v/>
       </c>
       <c r="B64" s="44" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C64" s="52">
         <v>0.2</v>
@@ -2126,7 +2126,7 @@
         <v/>
       </c>
       <c r="B65" s="44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C65" s="54">
         <v>0.7</v>
@@ -2149,7 +2149,7 @@
         <v/>
       </c>
       <c r="B66" s="44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C66" s="52">
         <v>0</v>
@@ -2171,7 +2171,7 @@
         <v/>
       </c>
       <c r="B67" s="44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C67" s="44"/>
       <c r="D67" s="50"/>
@@ -2186,7 +2186,7 @@
     <row r="68" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="67"/>
       <c r="B68" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C68" s="30"/>
       <c r="D68" s="80"/>
@@ -2200,10 +2200,10 @@
     </row>
     <row r="69" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="67" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C69" s="30"/>
       <c r="D69" s="80"/>
@@ -2222,10 +2222,10 @@
     </row>
     <row r="71" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A71" s="55" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B71" s="56" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C71" s="56"/>
       <c r="D71" s="56"/>
@@ -2247,15 +2247,15 @@
         <v>5</v>
       </c>
       <c r="B73" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="C73" s="103" t="s">
-        <v>53</v>
-      </c>
-      <c r="D73" s="103" t="s">
-        <v>54</v>
-      </c>
-      <c r="E73" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D73" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="E73" s="96" t="s">
         <v>25</v>
       </c>
       <c r="F73" s="5"/>
@@ -2263,7 +2263,7 @@
     <row r="74" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A74" s="7"/>
       <c r="B74" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C74" s="89">
         <f>1/(1+GK_NebenzeitenPersonal)</f>
@@ -2283,7 +2283,7 @@
     <row r="75" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A75" s="7"/>
       <c r="B75" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C75" s="89">
         <f>1/(1+GK_NebenzeitenGrundmaschine)</f>
@@ -2303,7 +2303,7 @@
     <row r="76" spans="1:6" s="3" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="55"/>
       <c r="B76" s="55" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C76" s="55"/>
       <c r="D76" s="74"/>
@@ -2328,13 +2328,13 @@
         <v>6</v>
       </c>
       <c r="B78" s="61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C78" s="62"/>
-      <c r="D78" s="104" t="s">
-        <v>54</v>
-      </c>
-      <c r="E78" s="105" t="s">
+      <c r="D78" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="E78" s="98" t="s">
         <v>25</v>
       </c>
       <c r="F78" s="64"/>
@@ -2342,7 +2342,7 @@
     <row r="79" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A79" s="62"/>
       <c r="B79" s="65" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C79" s="65"/>
       <c r="D79" s="66">
@@ -2367,13 +2367,13 @@
         <v>7</v>
       </c>
       <c r="B81" s="69" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C81" s="65"/>
-      <c r="D81" s="104" t="s">
-        <v>54</v>
-      </c>
-      <c r="E81" s="105" t="s">
+      <c r="D81" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="98" t="s">
         <v>25</v>
       </c>
       <c r="F81" s="64"/>
@@ -2381,7 +2381,7 @@
     <row r="82" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A82" s="62"/>
       <c r="B82" s="65" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C82" s="65"/>
       <c r="D82" s="66">
@@ -2405,10 +2405,10 @@
     </row>
     <row r="84" spans="1:6" s="4" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="70" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B84" s="71" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C84" s="71"/>
       <c r="D84" s="72"/>
@@ -2427,28 +2427,28 @@
     </row>
     <row r="86" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A86" s="70" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B86" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="C86" s="106" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" s="99" t="s">
+        <v>47</v>
+      </c>
+      <c r="D86" s="100" t="s">
+        <v>48</v>
+      </c>
+      <c r="E86" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="D86" s="107" t="s">
-        <v>50</v>
-      </c>
-      <c r="E86" s="108" t="s">
-        <v>51</v>
-      </c>
-      <c r="F86" s="108" t="s">
-        <v>67</v>
+      <c r="F86" s="101" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A87" s="76"/>
       <c r="B87" s="73" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C87" s="77">
         <v>0.8</v>
@@ -2468,7 +2468,7 @@
     <row r="88" spans="1:6" s="4" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="70"/>
       <c r="B88" s="71" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C88" s="83">
         <f>$E$84/C87</f>

</xml_diff>